<commit_message>
using lockdown for UK, Europe
</commit_message>
<xml_diff>
--- a/data/epidemiologypriors.xlsx
+++ b/data/epidemiologypriors.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aavattikutis/Git/covid-19/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661F0C2C-7038-3D47-9EED-6C1C54EA0423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F9E5FA-AA49-BC42-AFDF-BE0CA79C0AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{82EA345B-DE0F-0F4A-A92C-513349F5FA3E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{82EA345B-DE0F-0F4A-A92C-513349F5FA3E}"/>
   </bookViews>
   <sheets>
     <sheet name="mitigation" sheetId="1" r:id="rId1"/>
     <sheet name="mitigation sources" sheetId="2" r:id="rId2"/>
-    <sheet name="recovery_statistics" sheetId="3" r:id="rId3"/>
-    <sheet name="death_statistics" sheetId="4" r:id="rId4"/>
+    <sheet name="rec_death_statistics" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>region</t>
   </si>
@@ -249,6 +248,9 @@
   </si>
   <si>
     <t>https://www.medrxiv.org/content/10.1101/2020.04.01.20050138v1.full.pdf</t>
+  </si>
+  <si>
+    <t>lockdown</t>
   </si>
 </sst>
 </file>
@@ -256,7 +258,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -305,7 +307,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -623,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6314A468-2D72-3E45-805A-E1B0EE0F6FF6}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,7 +647,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>43900</v>
+        <v>43906</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -653,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>43900</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -661,7 +663,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>43902</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -669,7 +671,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>43903</v>
+        <v>43907</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -677,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>43896</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -685,7 +687,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>43899</v>
+        <v>43901</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -693,7 +695,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>43902</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -701,7 +703,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <v>43899</v>
+        <v>43904</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -709,7 +711,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>43900</v>
+        <v>43906</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -717,7 +719,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="4">
-        <v>43892</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -725,7 +727,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>43902</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1111,18 +1113,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF60C16-84DC-144F-8C7D-6E340746D0B6}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1137,23 +1144,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA69545-D5E7-FC44-9029-BCE0F650201F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A83E557-182E-3F42-99BA-C449A366DCB7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1168,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>63</v>
       </c>

</xml_diff>